<commit_message>
attributes training is modified
</commit_message>
<xml_diff>
--- a/results/mb_conv3_12branches_nowei_CA_network/attr_metrics.xlsx
+++ b/results/mb_conv3_12branches_nowei_CA_network/attr_metrics.xlsx
@@ -467,19 +467,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>0.8712260127067566</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>0.9262280464172363</v>
       </c>
       <c r="D2" t="n">
-        <v>0.9130434989929199</v>
+        <v>0.9063977599143982</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>0.8978849649429321</v>
       </c>
       <c r="F2" t="n">
-        <v>0.5</v>
+        <v>0.9083855152130127</v>
       </c>
     </row>
     <row r="3">
@@ -489,19 +489,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>0.6321839094161987</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>0.2801358103752136</v>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>0.9590293169021606</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>0.3882348537445068</v>
       </c>
       <c r="F3" t="n">
-        <v>0.5</v>
+        <v>0.6361019611358643</v>
       </c>
     </row>
     <row r="4">
@@ -511,19 +511,19 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>0.1084337383508682</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>0.0476190485060215</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>0.9799873828887939</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>0.06617604941129684</v>
       </c>
       <c r="F4" t="n">
-        <v>0.5</v>
+        <v>0.5208502411842346</v>
       </c>
     </row>
     <row r="5">
@@ -533,19 +533,19 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>0.8858789801597595</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>0.8713151812553406</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>0.8660573363304138</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>0.8785362243652344</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>0.8653949499130249</v>
       </c>
     </row>
     <row r="6">
@@ -555,19 +555,19 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>0.7549019455909729</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>0.8271835446357727</v>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>0.9255436658859253</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>0.7893911004066467</v>
       </c>
       <c r="F6" t="n">
-        <v>0.5</v>
+        <v>0.8863431811332703</v>
       </c>
     </row>
     <row r="7">
@@ -577,19 +577,19 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>0.6270411610603333</v>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>0.7082257270812988</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>0.8476993441581726</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>0.6651649475097656</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>0.7969042062759399</v>
       </c>
     </row>
     <row r="8">
@@ -599,19 +599,19 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>0.4575389921665192</v>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>0.2573099434375763</v>
       </c>
       <c r="D8" t="n">
-        <v>0.97826087474823</v>
+        <v>0.9153009653091431</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>0.3293819427490234</v>
       </c>
       <c r="F8" t="n">
-        <v>0.489130437374115</v>
+        <v>0.6152399182319641</v>
       </c>
     </row>
     <row r="9">
@@ -621,19 +621,19 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
+        <v>0.9366075396537781</v>
       </c>
       <c r="C9" t="n">
-        <v>0.97826087474823</v>
+        <v>0.973239541053772</v>
       </c>
       <c r="D9" t="n">
-        <v>0.97826087474823</v>
+        <v>0.9149070382118225</v>
       </c>
       <c r="E9" t="n">
-        <v>0.9890105128288269</v>
+        <v>0.9545717835426331</v>
       </c>
       <c r="F9" t="n">
-        <v>0.489130437374115</v>
+        <v>0.6148869395256042</v>
       </c>
     </row>
     <row r="10">
@@ -643,19 +643,19 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1</v>
+        <v>0.8953509330749512</v>
       </c>
       <c r="C10" t="n">
-        <v>1</v>
+        <v>0.92912358045578</v>
       </c>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>0.8481720685958862</v>
       </c>
       <c r="E10" t="n">
-        <v>0.9999995231628418</v>
+        <v>0.9119241833686829</v>
       </c>
       <c r="F10" t="n">
-        <v>0.5</v>
+        <v>0.6663520932197571</v>
       </c>
     </row>
     <row r="11">
@@ -665,19 +665,19 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0</v>
+        <v>0.3322683572769165</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>0.1522693932056427</v>
       </c>
       <c r="D11" t="n">
-        <v>1</v>
+        <v>0.9379136562347412</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>0.2088348865509033</v>
       </c>
       <c r="F11" t="n">
-        <v>0.5</v>
+        <v>0.5674328804016113</v>
       </c>
     </row>
     <row r="12">
@@ -687,19 +687,19 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0</v>
+        <v>0.1022727265954018</v>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>0.02564102597534657</v>
       </c>
       <c r="D12" t="n">
-        <v>1</v>
+        <v>0.9668294787406921</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>0.04100195690989494</v>
       </c>
       <c r="F12" t="n">
-        <v>0.5</v>
+        <v>0.5096198320388794</v>
       </c>
     </row>
     <row r="13">
@@ -709,19 +709,19 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0</v>
+        <v>0.4586597084999084</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>0.5759562849998474</v>
       </c>
       <c r="D13" t="n">
-        <v>1</v>
+        <v>0.9204223155975342</v>
       </c>
       <c r="E13" t="n">
-        <v>0</v>
+        <v>0.5106584429740906</v>
       </c>
       <c r="F13" t="n">
-        <v>0.5</v>
+        <v>0.7615707516670227</v>
       </c>
     </row>
     <row r="14">
@@ -731,19 +731,19 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.3999999165534973</v>
+        <v>0.5447154641151428</v>
       </c>
       <c r="C14" t="n">
-        <v>0.2499999701976776</v>
+        <v>0.07854630798101425</v>
       </c>
       <c r="D14" t="n">
-        <v>0.9021739363670349</v>
+        <v>0.9336590170860291</v>
       </c>
       <c r="E14" t="n">
-        <v>0.3076917827129364</v>
+        <v>0.1372948586940765</v>
       </c>
       <c r="F14" t="n">
-        <v>0.6071428656578064</v>
+        <v>0.5369080901145935</v>
       </c>
     </row>
     <row r="15">
@@ -753,19 +753,19 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.9999997019767761</v>
+        <v>0.8745366334915161</v>
       </c>
       <c r="C15" t="n">
-        <v>0.1874999850988388</v>
+        <v>0.7177627086639404</v>
       </c>
       <c r="D15" t="n">
-        <v>0.8586956262588501</v>
+        <v>0.8703120350837708</v>
       </c>
       <c r="E15" t="n">
-        <v>0.3157891929149628</v>
+        <v>0.7884314656257629</v>
       </c>
       <c r="F15" t="n">
-        <v>0.59375</v>
+        <v>0.8327499628067017</v>
       </c>
     </row>
     <row r="16">
@@ -775,19 +775,19 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.9999999403953552</v>
+        <v>0.8141592741012573</v>
       </c>
       <c r="C16" t="n">
-        <v>0.7333332896232605</v>
+        <v>0.7101754546165466</v>
       </c>
       <c r="D16" t="n">
-        <v>0.9130434989929199</v>
+        <v>0.9492594003677368</v>
       </c>
       <c r="E16" t="n">
-        <v>0.8461533188819885</v>
+        <v>0.7586202621459961</v>
       </c>
       <c r="F16" t="n">
-        <v>0.8666666746139526</v>
+        <v>0.8448365926742554</v>
       </c>
     </row>
     <row r="17">
@@ -797,19 +797,19 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1</v>
+        <v>0.973128616809845</v>
       </c>
       <c r="C17" t="n">
-        <v>1</v>
+        <v>0.8718830347061157</v>
       </c>
       <c r="D17" t="n">
-        <v>1</v>
+        <v>0.9860541820526123</v>
       </c>
       <c r="E17" t="n">
-        <v>0.9999995231628418</v>
+        <v>0.9197273850440979</v>
       </c>
       <c r="F17" t="n">
-        <v>1</v>
+        <v>0.9347271919250488</v>
       </c>
     </row>
     <row r="18">
@@ -819,19 +819,19 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0</v>
+        <v>0.787106454372406</v>
       </c>
       <c r="C18" t="n">
-        <v>0</v>
+        <v>0.6126021146774292</v>
       </c>
       <c r="D18" t="n">
-        <v>0.95652174949646</v>
+        <v>0.962653636932373</v>
       </c>
       <c r="E18" t="n">
-        <v>0</v>
+        <v>0.6889759302139282</v>
       </c>
       <c r="F18" t="n">
-        <v>0.47826087474823</v>
+        <v>0.8003019094467163</v>
       </c>
     </row>
     <row r="19">
@@ -841,19 +841,19 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0</v>
+        <v>0.6955307126045227</v>
       </c>
       <c r="C19" t="n">
-        <v>0</v>
+        <v>0.6505551934242249</v>
       </c>
       <c r="D19" t="n">
-        <v>1</v>
+        <v>0.9234951138496399</v>
       </c>
       <c r="E19" t="n">
-        <v>0</v>
+        <v>0.672291100025177</v>
       </c>
       <c r="F19" t="n">
-        <v>0.5</v>
+        <v>0.8057453036308289</v>
       </c>
     </row>
     <row r="20">
@@ -863,19 +863,19 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0</v>
+        <v>0.7321428656578064</v>
       </c>
       <c r="C20" t="n">
-        <v>0</v>
+        <v>0.4324894547462463</v>
       </c>
       <c r="D20" t="n">
-        <v>0.989130437374115</v>
+        <v>0.8915852308273315</v>
       </c>
       <c r="E20" t="n">
-        <v>0</v>
+        <v>0.5437661409378052</v>
       </c>
       <c r="F20" t="n">
-        <v>0.4945652186870575</v>
+        <v>0.7023507356643677</v>
       </c>
     </row>
     <row r="21">
@@ -885,19 +885,19 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0</v>
+        <v>0.8400900959968567</v>
       </c>
       <c r="C21" t="n">
-        <v>0</v>
+        <v>0.5088676810264587</v>
       </c>
       <c r="D21" t="n">
-        <v>1</v>
+        <v>0.966041624546051</v>
       </c>
       <c r="E21" t="n">
-        <v>0</v>
+        <v>0.6338143348693848</v>
       </c>
       <c r="F21" t="n">
-        <v>0.5</v>
+        <v>0.7514653205871582</v>
       </c>
     </row>
     <row r="22">
@@ -907,19 +907,19 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.9999998807907104</v>
+        <v>0.7851351499557495</v>
       </c>
       <c r="C22" t="n">
-        <v>0.8749998807907104</v>
+        <v>0.6755813956260681</v>
       </c>
       <c r="D22" t="n">
-        <v>0.989130437374115</v>
+        <v>0.9309801459312439</v>
       </c>
       <c r="E22" t="n">
-        <v>0.9333327412605286</v>
+        <v>0.7262495160102844</v>
       </c>
       <c r="F22" t="n">
-        <v>0.9374999403953552</v>
+        <v>0.8232992887496948</v>
       </c>
     </row>
     <row r="23">
@@ -929,19 +929,19 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.08695652335882187</v>
+        <v>0.320277214050293</v>
       </c>
       <c r="C23" t="n">
-        <v>0.9999998807907104</v>
+        <v>0.9582155346870422</v>
       </c>
       <c r="D23" t="n">
-        <v>0.08695652335882187</v>
+        <v>0.4795146584510803</v>
       </c>
       <c r="E23" t="n">
-        <v>0.1599998623132706</v>
+        <v>0.4800877869129181</v>
       </c>
       <c r="F23" t="n">
-        <v>0.4999999403953552</v>
+        <v>0.6387460231781006</v>
       </c>
     </row>
     <row r="24">
@@ -957,7 +957,7 @@
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>1</v>
+        <v>0.9886542558670044</v>
       </c>
       <c r="E24" t="n">
         <v>0</v>
@@ -979,7 +979,7 @@
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>0.9130434989929199</v>
+        <v>0.7605578303337097</v>
       </c>
       <c r="E25" t="n">
         <v>0</v>
@@ -995,19 +995,19 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0</v>
+        <v>0.7305143475532532</v>
       </c>
       <c r="C26" t="n">
-        <v>0</v>
+        <v>0.5026053190231323</v>
       </c>
       <c r="D26" t="n">
-        <v>0.08695652335882187</v>
+        <v>0.7522060871124268</v>
       </c>
       <c r="E26" t="n">
-        <v>0</v>
+        <v>0.5954979062080383</v>
       </c>
       <c r="F26" t="n">
-        <v>0.4999999403953552</v>
+        <v>0.6984953284263611</v>
       </c>
     </row>
     <row r="27">
@@ -1017,19 +1017,19 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.4239130318164825</v>
+        <v>0.9261554479598999</v>
       </c>
       <c r="C27" t="n">
-        <v>1</v>
+        <v>0.8891918659210205</v>
       </c>
       <c r="D27" t="n">
-        <v>0.4239130318164825</v>
+        <v>0.9422470927238464</v>
       </c>
       <c r="E27" t="n">
-        <v>0.5954194664955139</v>
+        <v>0.907296895980835</v>
       </c>
       <c r="F27" t="n">
-        <v>0.5</v>
+        <v>0.9280794262886047</v>
       </c>
     </row>
     <row r="28">
@@ -1039,19 +1039,19 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0</v>
+        <v>0.891465425491333</v>
       </c>
       <c r="C28" t="n">
-        <v>0</v>
+        <v>0.9216910004615784</v>
       </c>
       <c r="D28" t="n">
-        <v>0.4239130318164825</v>
+        <v>0.8941853046417236</v>
       </c>
       <c r="E28" t="n">
-        <v>0</v>
+        <v>0.9063258171081543</v>
       </c>
       <c r="F28" t="n">
-        <v>0.5</v>
+        <v>0.8907586336135864</v>
       </c>
     </row>
     <row r="29">
@@ -1061,19 +1061,19 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0</v>
+        <v>0.7517961859703064</v>
       </c>
       <c r="C29" t="n">
-        <v>0</v>
+        <v>0.718028724193573</v>
       </c>
       <c r="D29" t="n">
-        <v>1</v>
+        <v>0.9344468712806702</v>
       </c>
       <c r="E29" t="n">
-        <v>0</v>
+        <v>0.7345240712165833</v>
       </c>
       <c r="F29" t="n">
-        <v>0.5</v>
+        <v>0.8418802618980408</v>
       </c>
     </row>
     <row r="30">
@@ -1083,19 +1083,19 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0</v>
+        <v>0.5366747975349426</v>
       </c>
       <c r="C30" t="n">
-        <v>0</v>
+        <v>0.5028637051582336</v>
       </c>
       <c r="D30" t="n">
-        <v>0.9130434989929199</v>
+        <v>0.9359439015388489</v>
       </c>
       <c r="E30" t="n">
-        <v>0</v>
+        <v>0.519218921661377</v>
       </c>
       <c r="F30" t="n">
-        <v>0.5</v>
+        <v>0.7353983521461487</v>
       </c>
     </row>
     <row r="31">
@@ -1105,19 +1105,19 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0</v>
+        <v>0.3299180269241333</v>
       </c>
       <c r="C31" t="n">
-        <v>0</v>
+        <v>0.574999988079071</v>
       </c>
       <c r="D31" t="n">
-        <v>0.989130437374115</v>
+        <v>0.9648597836494446</v>
       </c>
       <c r="E31" t="n">
-        <v>0</v>
+        <v>0.4192703664302826</v>
       </c>
       <c r="F31" t="n">
-        <v>0.4945652186870575</v>
+        <v>0.774327278137207</v>
       </c>
     </row>
     <row r="32">
@@ -1127,19 +1127,19 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0</v>
+        <v>0.4123989343643188</v>
       </c>
       <c r="C32" t="n">
-        <v>0</v>
+        <v>0.3903061151504517</v>
       </c>
       <c r="D32" t="n">
-        <v>0.95652174949646</v>
+        <v>0.9639930725097656</v>
       </c>
       <c r="E32" t="n">
-        <v>0</v>
+        <v>0.4010479748249054</v>
       </c>
       <c r="F32" t="n">
-        <v>0.47826087474823</v>
+        <v>0.6862912774085999</v>
       </c>
     </row>
     <row r="33">
@@ -1149,19 +1149,19 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0</v>
+        <v>0.5658436417579651</v>
       </c>
       <c r="C33" t="n">
-        <v>0</v>
+        <v>0.3450439274311066</v>
       </c>
       <c r="D33" t="n">
-        <v>0.72826087474823</v>
+        <v>0.9422470927238464</v>
       </c>
       <c r="E33" t="n">
-        <v>0</v>
+        <v>0.4286822974681854</v>
       </c>
       <c r="F33" t="n">
-        <v>0.364130437374115</v>
+        <v>0.6636527180671692</v>
       </c>
     </row>
     <row r="34">
@@ -1171,19 +1171,19 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.04999999701976776</v>
+        <v>0.3682926893234253</v>
       </c>
       <c r="C34" t="n">
-        <v>0.3333332240581512</v>
+        <v>0.4026666581630707</v>
       </c>
       <c r="D34" t="n">
-        <v>0.77173912525177</v>
+        <v>0.9619445204734802</v>
       </c>
       <c r="E34" t="n">
-        <v>0.08695628494024277</v>
+        <v>0.3847128450870514</v>
       </c>
       <c r="F34" t="n">
-        <v>0.5599250197410583</v>
+        <v>0.6908193826675415</v>
       </c>
     </row>
     <row r="35">
@@ -1193,19 +1193,19 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.07692307233810425</v>
+        <v>0.7723866105079651</v>
       </c>
       <c r="C35" t="n">
-        <v>0.07692307233810425</v>
+        <v>0.6938341856002808</v>
       </c>
       <c r="D35" t="n">
-        <v>0.47826087474823</v>
+        <v>0.8864639401435852</v>
       </c>
       <c r="E35" t="n">
-        <v>0.07692257314920425</v>
+        <v>0.7310056686401367</v>
       </c>
       <c r="F35" t="n">
-        <v>0.3566433489322662</v>
+        <v>0.8176870942115784</v>
       </c>
     </row>
     <row r="36">
@@ -1215,19 +1215,19 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0</v>
+        <v>0.5500413775444031</v>
       </c>
       <c r="C36" t="n">
-        <v>0</v>
+        <v>0.5657167434692383</v>
       </c>
       <c r="D36" t="n">
-        <v>0.8913043737411499</v>
+        <v>0.833832323551178</v>
       </c>
       <c r="E36" t="n">
-        <v>0</v>
+        <v>0.5577684640884399</v>
       </c>
       <c r="F36" t="n">
-        <v>0.488095223903656</v>
+        <v>0.7302522659301758</v>
       </c>
     </row>
     <row r="37">
@@ -1243,7 +1243,7 @@
         <v>0</v>
       </c>
       <c r="D37" t="n">
-        <v>1</v>
+        <v>0.9913331270217896</v>
       </c>
       <c r="E37" t="n">
         <v>0</v>
@@ -1259,19 +1259,19 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>0.2857142686843872</v>
+        <v>0.8029423356056213</v>
       </c>
       <c r="C38" t="n">
-        <v>0.08510638028383255</v>
+        <v>0.885189950466156</v>
       </c>
       <c r="D38" t="n">
-        <v>0.4239130318164825</v>
+        <v>0.8774030804634094</v>
       </c>
       <c r="E38" t="n">
-        <v>0.1311471909284592</v>
+        <v>0.8420620560646057</v>
       </c>
       <c r="F38" t="n">
-        <v>0.4314420819282532</v>
+        <v>0.8790176510810852</v>
       </c>
     </row>
     <row r="39">
@@ -1281,19 +1281,19 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>0.8152173757553101</v>
+        <v>0.82596355676651</v>
       </c>
       <c r="C39" t="n">
-        <v>1</v>
+        <v>0.8098770976066589</v>
       </c>
       <c r="D39" t="n">
-        <v>0.8152173757553101</v>
+        <v>0.7548061609268188</v>
       </c>
       <c r="E39" t="n">
-        <v>0.8982031345367432</v>
+        <v>0.8178407549858093</v>
       </c>
       <c r="F39" t="n">
-        <v>0.5</v>
+        <v>0.7239252328872681</v>
       </c>
     </row>
     <row r="40">
@@ -1303,19 +1303,19 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>0</v>
+        <v>0.5933352112770081</v>
       </c>
       <c r="C40" t="n">
-        <v>0</v>
+        <v>0.6163097620010376</v>
       </c>
       <c r="D40" t="n">
-        <v>0.8260869383811951</v>
+        <v>0.7834856510162354</v>
       </c>
       <c r="E40" t="n">
-        <v>0</v>
+        <v>0.6046038269996643</v>
       </c>
       <c r="F40" t="n">
-        <v>0.5</v>
+        <v>0.730593740940094</v>
       </c>
     </row>
     <row r="41">
@@ -1325,19 +1325,19 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>0</v>
+        <v>0.5440115332603455</v>
       </c>
       <c r="C41" t="n">
-        <v>0</v>
+        <v>0.5791090726852417</v>
       </c>
       <c r="D41" t="n">
-        <v>0.989130437374115</v>
+        <v>0.953514039516449</v>
       </c>
       <c r="E41" t="n">
-        <v>0</v>
+        <v>0.5610114932060242</v>
       </c>
       <c r="F41" t="n">
-        <v>0.5</v>
+        <v>0.7764326930046082</v>
       </c>
     </row>
     <row r="42">
@@ -1347,19 +1347,19 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>0.555555522441864</v>
+        <v>0.588320791721344</v>
       </c>
       <c r="C42" t="n">
-        <v>0.8823528289794922</v>
+        <v>0.5980295538902283</v>
       </c>
       <c r="D42" t="n">
-        <v>0.8478260636329651</v>
+        <v>0.737551212310791</v>
       </c>
       <c r="E42" t="n">
-        <v>0.6818176507949829</v>
+        <v>0.5931349992752075</v>
       </c>
       <c r="F42" t="n">
-        <v>0.8611763715744019</v>
+        <v>0.7006019353866577</v>
       </c>
     </row>
     <row r="43">
@@ -1369,19 +1369,19 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>0.7777776718139648</v>
+        <v>0.4675492346286774</v>
       </c>
       <c r="C43" t="n">
-        <v>0.8749998807907104</v>
+        <v>0.6156462430953979</v>
       </c>
       <c r="D43" t="n">
-        <v>0.967391312122345</v>
+        <v>0.7988496422767639</v>
       </c>
       <c r="E43" t="n">
-        <v>0.8235287666320801</v>
+        <v>0.5314732193946838</v>
       </c>
       <c r="F43" t="n">
-        <v>0.9255951642990112</v>
+        <v>0.7280842065811157</v>
       </c>
     </row>
     <row r="44">
@@ -1391,19 +1391,19 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>0.8461537957191467</v>
+        <v>0.5450361371040344</v>
       </c>
       <c r="C44" t="n">
-        <v>0.3793103098869324</v>
+        <v>0.2902660965919495</v>
       </c>
       <c r="D44" t="n">
-        <v>0.782608687877655</v>
+        <v>0.7857705354690552</v>
       </c>
       <c r="E44" t="n">
-        <v>0.5238090753555298</v>
+        <v>0.3787977695465088</v>
       </c>
       <c r="F44" t="n">
-        <v>0.6737821102142334</v>
+        <v>0.6099561452865601</v>
       </c>
     </row>
     <row r="45">
@@ -1413,19 +1413,19 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>0.8372092843055725</v>
+        <v>0.6148973703384399</v>
       </c>
       <c r="C45" t="n">
-        <v>0.9473684430122375</v>
+        <v>0.7100643515586853</v>
       </c>
       <c r="D45" t="n">
-        <v>0.9021739363670349</v>
+        <v>0.8021588325500488</v>
       </c>
       <c r="E45" t="n">
-        <v>0.888888418674469</v>
+        <v>0.6590626835823059</v>
       </c>
       <c r="F45" t="n">
-        <v>0.9088693857192993</v>
+        <v>0.7730826139450073</v>
       </c>
     </row>
     <row r="46">
@@ -1435,19 +1435,19 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>0</v>
+        <v>0.3636363446712494</v>
       </c>
       <c r="C46" t="n">
-        <v>0</v>
+        <v>0.1176470592617989</v>
       </c>
       <c r="D46" t="n">
-        <v>1</v>
+        <v>0.9970847964286804</v>
       </c>
       <c r="E46" t="n">
-        <v>0</v>
+        <v>0.1777773946523666</v>
       </c>
       <c r="F46" t="n">
-        <v>0.5</v>
+        <v>0.5585470199584961</v>
       </c>
     </row>
     <row r="47">
@@ -1457,19 +1457,19 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>1</v>
+        <v>0.935258150100708</v>
       </c>
       <c r="C47" t="n">
-        <v>1</v>
+        <v>0.8556617498397827</v>
       </c>
       <c r="D47" t="n">
-        <v>1</v>
+        <v>0.8220926523208618</v>
       </c>
       <c r="E47" t="n">
-        <v>0.9999995231628418</v>
+        <v>0.8936906456947327</v>
       </c>
       <c r="F47" t="n">
-        <v>0.5</v>
+        <v>0.7225183844566345</v>
       </c>
     </row>
     <row r="48">
@@ -1479,19 +1479,19 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>0</v>
+        <v>0.3549663722515106</v>
       </c>
       <c r="C48" t="n">
-        <v>0</v>
+        <v>0.6056718230247498</v>
       </c>
       <c r="D48" t="n">
-        <v>1</v>
+        <v>0.8255594372749329</v>
       </c>
       <c r="E48" t="n">
-        <v>0</v>
+        <v>0.4476043283939362</v>
       </c>
       <c r="F48" t="n">
-        <v>0.5</v>
+        <v>0.7301394939422607</v>
       </c>
     </row>
     <row r="49">
@@ -1507,13 +1507,13 @@
         <v>0</v>
       </c>
       <c r="D49" t="n">
-        <v>1</v>
+        <v>0.9928301572799683</v>
       </c>
       <c r="E49" t="n">
         <v>0</v>
       </c>
       <c r="F49" t="n">
-        <v>0.5</v>
+        <v>0.4997620284557343</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
a function to saving in csv is added
</commit_message>
<xml_diff>
--- a/results/mb_conv3_12branches_nowei_CA_network/attr_metrics.xlsx
+++ b/results/mb_conv3_12branches_nowei_CA_network/attr_metrics.xlsx
@@ -467,19 +467,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.8712260127067566</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>0.9262280464172363</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0.9063977599143982</v>
+        <v>0.9130434989929199</v>
       </c>
       <c r="E2" t="n">
-        <v>0.8978849649429321</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0.9083855152130127</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="3">
@@ -489,19 +489,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.6321839094161987</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>0.2801358103752136</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>0.9590293169021606</v>
+        <v>1</v>
       </c>
       <c r="E3" t="n">
-        <v>0.3882348537445068</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>0.6361019611358643</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="4">
@@ -511,19 +511,19 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.1084337383508682</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0476190485060215</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0.9799873828887939</v>
+        <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>0.06617604941129684</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.5208502411842346</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="5">
@@ -533,19 +533,19 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.8858789801597595</v>
+        <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>0.8713151812553406</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0.8660573363304138</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>0.8785362243652344</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>0.8653949499130249</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -555,19 +555,19 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.7549019455909729</v>
+        <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>0.8271835446357727</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>0.9255436658859253</v>
+        <v>1</v>
       </c>
       <c r="E6" t="n">
-        <v>0.7893911004066467</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>0.8863431811332703</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="7">
@@ -577,19 +577,19 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.6270411610603333</v>
+        <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>0.7082257270812988</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>0.8476993441581726</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>0.6651649475097656</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>0.7969042062759399</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -599,19 +599,19 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.4575389921665192</v>
+        <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>0.2573099434375763</v>
+        <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>0.9153009653091431</v>
+        <v>0.97826087474823</v>
       </c>
       <c r="E8" t="n">
-        <v>0.3293819427490234</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>0.6152399182319641</v>
+        <v>0.489130437374115</v>
       </c>
     </row>
     <row r="9">
@@ -621,19 +621,19 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.9366075396537781</v>
+        <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>0.973239541053772</v>
+        <v>0.97826087474823</v>
       </c>
       <c r="D9" t="n">
-        <v>0.9149070382118225</v>
+        <v>0.97826087474823</v>
       </c>
       <c r="E9" t="n">
-        <v>0.9545717835426331</v>
+        <v>0.9890105128288269</v>
       </c>
       <c r="F9" t="n">
-        <v>0.6148869395256042</v>
+        <v>0.489130437374115</v>
       </c>
     </row>
     <row r="10">
@@ -643,19 +643,19 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.8953509330749512</v>
+        <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>0.92912358045578</v>
+        <v>1</v>
       </c>
       <c r="D10" t="n">
-        <v>0.8481720685958862</v>
+        <v>1</v>
       </c>
       <c r="E10" t="n">
-        <v>0.9119241833686829</v>
+        <v>0.9999995231628418</v>
       </c>
       <c r="F10" t="n">
-        <v>0.6663520932197571</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="11">
@@ -665,19 +665,19 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.3322683572769165</v>
+        <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>0.1522693932056427</v>
+        <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>0.9379136562347412</v>
+        <v>1</v>
       </c>
       <c r="E11" t="n">
-        <v>0.2088348865509033</v>
+        <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>0.5674328804016113</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="12">
@@ -687,19 +687,19 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.1022727265954018</v>
+        <v>0</v>
       </c>
       <c r="C12" t="n">
-        <v>0.02564102597534657</v>
+        <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>0.9668294787406921</v>
+        <v>1</v>
       </c>
       <c r="E12" t="n">
-        <v>0.04100195690989494</v>
+        <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>0.5096198320388794</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="13">
@@ -709,19 +709,19 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.4586597084999084</v>
+        <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>0.5759562849998474</v>
+        <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>0.9204223155975342</v>
+        <v>1</v>
       </c>
       <c r="E13" t="n">
-        <v>0.5106584429740906</v>
+        <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>0.7615707516670227</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="14">
@@ -731,19 +731,19 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.5447154641151428</v>
+        <v>0.3999999165534973</v>
       </c>
       <c r="C14" t="n">
-        <v>0.07854630798101425</v>
+        <v>0.2499999701976776</v>
       </c>
       <c r="D14" t="n">
-        <v>0.9336590170860291</v>
+        <v>0.9021739363670349</v>
       </c>
       <c r="E14" t="n">
-        <v>0.1372948586940765</v>
+        <v>0.3076917827129364</v>
       </c>
       <c r="F14" t="n">
-        <v>0.5369080901145935</v>
+        <v>0.6071428656578064</v>
       </c>
     </row>
     <row r="15">
@@ -753,19 +753,19 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.8745366334915161</v>
+        <v>0.9999997019767761</v>
       </c>
       <c r="C15" t="n">
-        <v>0.7177627086639404</v>
+        <v>0.1874999850988388</v>
       </c>
       <c r="D15" t="n">
-        <v>0.8703120350837708</v>
+        <v>0.8586956262588501</v>
       </c>
       <c r="E15" t="n">
-        <v>0.7884314656257629</v>
+        <v>0.3157891929149628</v>
       </c>
       <c r="F15" t="n">
-        <v>0.8327499628067017</v>
+        <v>0.59375</v>
       </c>
     </row>
     <row r="16">
@@ -775,19 +775,19 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.8141592741012573</v>
+        <v>0.9999999403953552</v>
       </c>
       <c r="C16" t="n">
-        <v>0.7101754546165466</v>
+        <v>0.7333332896232605</v>
       </c>
       <c r="D16" t="n">
-        <v>0.9492594003677368</v>
+        <v>0.9130434989929199</v>
       </c>
       <c r="E16" t="n">
-        <v>0.7586202621459961</v>
+        <v>0.8461533188819885</v>
       </c>
       <c r="F16" t="n">
-        <v>0.8448365926742554</v>
+        <v>0.8666666746139526</v>
       </c>
     </row>
     <row r="17">
@@ -797,19 +797,19 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.973128616809845</v>
+        <v>1</v>
       </c>
       <c r="C17" t="n">
-        <v>0.8718830347061157</v>
+        <v>1</v>
       </c>
       <c r="D17" t="n">
-        <v>0.9860541820526123</v>
+        <v>1</v>
       </c>
       <c r="E17" t="n">
-        <v>0.9197273850440979</v>
+        <v>0.9999995231628418</v>
       </c>
       <c r="F17" t="n">
-        <v>0.9347271919250488</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
@@ -819,19 +819,19 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.787106454372406</v>
+        <v>0</v>
       </c>
       <c r="C18" t="n">
-        <v>0.6126021146774292</v>
+        <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>0.962653636932373</v>
+        <v>0.95652174949646</v>
       </c>
       <c r="E18" t="n">
-        <v>0.6889759302139282</v>
+        <v>0</v>
       </c>
       <c r="F18" t="n">
-        <v>0.8003019094467163</v>
+        <v>0.47826087474823</v>
       </c>
     </row>
     <row r="19">
@@ -841,19 +841,19 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.6955307126045227</v>
+        <v>0</v>
       </c>
       <c r="C19" t="n">
-        <v>0.6505551934242249</v>
+        <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>0.9234951138496399</v>
+        <v>1</v>
       </c>
       <c r="E19" t="n">
-        <v>0.672291100025177</v>
+        <v>0</v>
       </c>
       <c r="F19" t="n">
-        <v>0.8057453036308289</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="20">
@@ -863,19 +863,19 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.7321428656578064</v>
+        <v>0</v>
       </c>
       <c r="C20" t="n">
-        <v>0.4324894547462463</v>
+        <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>0.8915852308273315</v>
+        <v>0.989130437374115</v>
       </c>
       <c r="E20" t="n">
-        <v>0.5437661409378052</v>
+        <v>0</v>
       </c>
       <c r="F20" t="n">
-        <v>0.7023507356643677</v>
+        <v>0.4945652186870575</v>
       </c>
     </row>
     <row r="21">
@@ -885,19 +885,19 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.8400900959968567</v>
+        <v>0</v>
       </c>
       <c r="C21" t="n">
-        <v>0.5088676810264587</v>
+        <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>0.966041624546051</v>
+        <v>1</v>
       </c>
       <c r="E21" t="n">
-        <v>0.6338143348693848</v>
+        <v>0</v>
       </c>
       <c r="F21" t="n">
-        <v>0.7514653205871582</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="22">
@@ -907,19 +907,19 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.7851351499557495</v>
+        <v>0.9999998807907104</v>
       </c>
       <c r="C22" t="n">
-        <v>0.6755813956260681</v>
+        <v>0.8749998807907104</v>
       </c>
       <c r="D22" t="n">
-        <v>0.9309801459312439</v>
+        <v>0.989130437374115</v>
       </c>
       <c r="E22" t="n">
-        <v>0.7262495160102844</v>
+        <v>0.9333327412605286</v>
       </c>
       <c r="F22" t="n">
-        <v>0.8232992887496948</v>
+        <v>0.9374999403953552</v>
       </c>
     </row>
     <row r="23">
@@ -929,19 +929,19 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.320277214050293</v>
+        <v>0.08695652335882187</v>
       </c>
       <c r="C23" t="n">
-        <v>0.9582155346870422</v>
+        <v>0.9999998807907104</v>
       </c>
       <c r="D23" t="n">
-        <v>0.4795146584510803</v>
+        <v>0.08695652335882187</v>
       </c>
       <c r="E23" t="n">
-        <v>0.4800877869129181</v>
+        <v>0.1599998623132706</v>
       </c>
       <c r="F23" t="n">
-        <v>0.6387460231781006</v>
+        <v>0.4999999403953552</v>
       </c>
     </row>
     <row r="24">
@@ -957,7 +957,7 @@
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>0.9886542558670044</v>
+        <v>1</v>
       </c>
       <c r="E24" t="n">
         <v>0</v>
@@ -979,7 +979,7 @@
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>0.7605578303337097</v>
+        <v>0.9130434989929199</v>
       </c>
       <c r="E25" t="n">
         <v>0</v>
@@ -995,19 +995,19 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.7305143475532532</v>
+        <v>0</v>
       </c>
       <c r="C26" t="n">
-        <v>0.5026053190231323</v>
+        <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>0.7522060871124268</v>
+        <v>0.08695652335882187</v>
       </c>
       <c r="E26" t="n">
-        <v>0.5954979062080383</v>
+        <v>0</v>
       </c>
       <c r="F26" t="n">
-        <v>0.6984953284263611</v>
+        <v>0.4999999403953552</v>
       </c>
     </row>
     <row r="27">
@@ -1017,19 +1017,19 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.9261554479598999</v>
+        <v>0.4239130318164825</v>
       </c>
       <c r="C27" t="n">
-        <v>0.8891918659210205</v>
+        <v>1</v>
       </c>
       <c r="D27" t="n">
-        <v>0.9422470927238464</v>
+        <v>0.4239130318164825</v>
       </c>
       <c r="E27" t="n">
-        <v>0.907296895980835</v>
+        <v>0.5954194664955139</v>
       </c>
       <c r="F27" t="n">
-        <v>0.9280794262886047</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="28">
@@ -1039,19 +1039,19 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.891465425491333</v>
+        <v>0</v>
       </c>
       <c r="C28" t="n">
-        <v>0.9216910004615784</v>
+        <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>0.8941853046417236</v>
+        <v>0.4239130318164825</v>
       </c>
       <c r="E28" t="n">
-        <v>0.9063258171081543</v>
+        <v>0</v>
       </c>
       <c r="F28" t="n">
-        <v>0.8907586336135864</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="29">
@@ -1061,19 +1061,19 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.7517961859703064</v>
+        <v>0</v>
       </c>
       <c r="C29" t="n">
-        <v>0.718028724193573</v>
+        <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>0.9344468712806702</v>
+        <v>1</v>
       </c>
       <c r="E29" t="n">
-        <v>0.7345240712165833</v>
+        <v>0</v>
       </c>
       <c r="F29" t="n">
-        <v>0.8418802618980408</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="30">
@@ -1083,19 +1083,19 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.5366747975349426</v>
+        <v>0</v>
       </c>
       <c r="C30" t="n">
-        <v>0.5028637051582336</v>
+        <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>0.9359439015388489</v>
+        <v>0.9130434989929199</v>
       </c>
       <c r="E30" t="n">
-        <v>0.519218921661377</v>
+        <v>0</v>
       </c>
       <c r="F30" t="n">
-        <v>0.7353983521461487</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="31">
@@ -1105,19 +1105,19 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.3299180269241333</v>
+        <v>0</v>
       </c>
       <c r="C31" t="n">
-        <v>0.574999988079071</v>
+        <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>0.9648597836494446</v>
+        <v>0.989130437374115</v>
       </c>
       <c r="E31" t="n">
-        <v>0.4192703664302826</v>
+        <v>0</v>
       </c>
       <c r="F31" t="n">
-        <v>0.774327278137207</v>
+        <v>0.4945652186870575</v>
       </c>
     </row>
     <row r="32">
@@ -1127,19 +1127,19 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.4123989343643188</v>
+        <v>0</v>
       </c>
       <c r="C32" t="n">
-        <v>0.3903061151504517</v>
+        <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>0.9639930725097656</v>
+        <v>0.95652174949646</v>
       </c>
       <c r="E32" t="n">
-        <v>0.4010479748249054</v>
+        <v>0</v>
       </c>
       <c r="F32" t="n">
-        <v>0.6862912774085999</v>
+        <v>0.47826087474823</v>
       </c>
     </row>
     <row r="33">
@@ -1149,19 +1149,19 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.5658436417579651</v>
+        <v>0</v>
       </c>
       <c r="C33" t="n">
-        <v>0.3450439274311066</v>
+        <v>0</v>
       </c>
       <c r="D33" t="n">
-        <v>0.9422470927238464</v>
+        <v>0.72826087474823</v>
       </c>
       <c r="E33" t="n">
-        <v>0.4286822974681854</v>
+        <v>0</v>
       </c>
       <c r="F33" t="n">
-        <v>0.6636527180671692</v>
+        <v>0.364130437374115</v>
       </c>
     </row>
     <row r="34">
@@ -1171,19 +1171,19 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.3682926893234253</v>
+        <v>0.04999999701976776</v>
       </c>
       <c r="C34" t="n">
-        <v>0.4026666581630707</v>
+        <v>0.3333332240581512</v>
       </c>
       <c r="D34" t="n">
-        <v>0.9619445204734802</v>
+        <v>0.77173912525177</v>
       </c>
       <c r="E34" t="n">
-        <v>0.3847128450870514</v>
+        <v>0.08695628494024277</v>
       </c>
       <c r="F34" t="n">
-        <v>0.6908193826675415</v>
+        <v>0.5599250197410583</v>
       </c>
     </row>
     <row r="35">
@@ -1193,19 +1193,19 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.7723866105079651</v>
+        <v>0.07692307233810425</v>
       </c>
       <c r="C35" t="n">
-        <v>0.6938341856002808</v>
+        <v>0.07692307233810425</v>
       </c>
       <c r="D35" t="n">
-        <v>0.8864639401435852</v>
+        <v>0.47826087474823</v>
       </c>
       <c r="E35" t="n">
-        <v>0.7310056686401367</v>
+        <v>0.07692257314920425</v>
       </c>
       <c r="F35" t="n">
-        <v>0.8176870942115784</v>
+        <v>0.3566433489322662</v>
       </c>
     </row>
     <row r="36">
@@ -1215,19 +1215,19 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0.5500413775444031</v>
+        <v>0</v>
       </c>
       <c r="C36" t="n">
-        <v>0.5657167434692383</v>
+        <v>0</v>
       </c>
       <c r="D36" t="n">
-        <v>0.833832323551178</v>
+        <v>0.8913043737411499</v>
       </c>
       <c r="E36" t="n">
-        <v>0.5577684640884399</v>
+        <v>0</v>
       </c>
       <c r="F36" t="n">
-        <v>0.7302522659301758</v>
+        <v>0.488095223903656</v>
       </c>
     </row>
     <row r="37">
@@ -1243,7 +1243,7 @@
         <v>0</v>
       </c>
       <c r="D37" t="n">
-        <v>0.9913331270217896</v>
+        <v>1</v>
       </c>
       <c r="E37" t="n">
         <v>0</v>
@@ -1259,19 +1259,19 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>0.8029423356056213</v>
+        <v>0.2857142686843872</v>
       </c>
       <c r="C38" t="n">
-        <v>0.885189950466156</v>
+        <v>0.08510638028383255</v>
       </c>
       <c r="D38" t="n">
-        <v>0.8774030804634094</v>
+        <v>0.4239130318164825</v>
       </c>
       <c r="E38" t="n">
-        <v>0.8420620560646057</v>
+        <v>0.1311471909284592</v>
       </c>
       <c r="F38" t="n">
-        <v>0.8790176510810852</v>
+        <v>0.4314420819282532</v>
       </c>
     </row>
     <row r="39">
@@ -1281,19 +1281,19 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>0.82596355676651</v>
+        <v>0.8152173757553101</v>
       </c>
       <c r="C39" t="n">
-        <v>0.8098770976066589</v>
+        <v>1</v>
       </c>
       <c r="D39" t="n">
-        <v>0.7548061609268188</v>
+        <v>0.8152173757553101</v>
       </c>
       <c r="E39" t="n">
-        <v>0.8178407549858093</v>
+        <v>0.8982031345367432</v>
       </c>
       <c r="F39" t="n">
-        <v>0.7239252328872681</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="40">
@@ -1303,19 +1303,19 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>0.5933352112770081</v>
+        <v>0</v>
       </c>
       <c r="C40" t="n">
-        <v>0.6163097620010376</v>
+        <v>0</v>
       </c>
       <c r="D40" t="n">
-        <v>0.7834856510162354</v>
+        <v>0.8260869383811951</v>
       </c>
       <c r="E40" t="n">
-        <v>0.6046038269996643</v>
+        <v>0</v>
       </c>
       <c r="F40" t="n">
-        <v>0.730593740940094</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="41">
@@ -1325,19 +1325,19 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>0.5440115332603455</v>
+        <v>0</v>
       </c>
       <c r="C41" t="n">
-        <v>0.5791090726852417</v>
+        <v>0</v>
       </c>
       <c r="D41" t="n">
-        <v>0.953514039516449</v>
+        <v>0.989130437374115</v>
       </c>
       <c r="E41" t="n">
-        <v>0.5610114932060242</v>
+        <v>0</v>
       </c>
       <c r="F41" t="n">
-        <v>0.7764326930046082</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="42">
@@ -1347,19 +1347,19 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>0.588320791721344</v>
+        <v>0.555555522441864</v>
       </c>
       <c r="C42" t="n">
-        <v>0.5980295538902283</v>
+        <v>0.8823528289794922</v>
       </c>
       <c r="D42" t="n">
-        <v>0.737551212310791</v>
+        <v>0.8478260636329651</v>
       </c>
       <c r="E42" t="n">
-        <v>0.5931349992752075</v>
+        <v>0.6818176507949829</v>
       </c>
       <c r="F42" t="n">
-        <v>0.7006019353866577</v>
+        <v>0.8611763715744019</v>
       </c>
     </row>
     <row r="43">
@@ -1369,19 +1369,19 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>0.4675492346286774</v>
+        <v>0.7777776718139648</v>
       </c>
       <c r="C43" t="n">
-        <v>0.6156462430953979</v>
+        <v>0.8749998807907104</v>
       </c>
       <c r="D43" t="n">
-        <v>0.7988496422767639</v>
+        <v>0.967391312122345</v>
       </c>
       <c r="E43" t="n">
-        <v>0.5314732193946838</v>
+        <v>0.8235287666320801</v>
       </c>
       <c r="F43" t="n">
-        <v>0.7280842065811157</v>
+        <v>0.9255951642990112</v>
       </c>
     </row>
     <row r="44">
@@ -1391,19 +1391,19 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>0.5450361371040344</v>
+        <v>0.8461537957191467</v>
       </c>
       <c r="C44" t="n">
-        <v>0.2902660965919495</v>
+        <v>0.3793103098869324</v>
       </c>
       <c r="D44" t="n">
-        <v>0.7857705354690552</v>
+        <v>0.782608687877655</v>
       </c>
       <c r="E44" t="n">
-        <v>0.3787977695465088</v>
+        <v>0.5238090753555298</v>
       </c>
       <c r="F44" t="n">
-        <v>0.6099561452865601</v>
+        <v>0.6737821102142334</v>
       </c>
     </row>
     <row r="45">
@@ -1413,19 +1413,19 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>0.6148973703384399</v>
+        <v>0.8372092843055725</v>
       </c>
       <c r="C45" t="n">
-        <v>0.7100643515586853</v>
+        <v>0.9473684430122375</v>
       </c>
       <c r="D45" t="n">
-        <v>0.8021588325500488</v>
+        <v>0.9021739363670349</v>
       </c>
       <c r="E45" t="n">
-        <v>0.6590626835823059</v>
+        <v>0.888888418674469</v>
       </c>
       <c r="F45" t="n">
-        <v>0.7730826139450073</v>
+        <v>0.9088693857192993</v>
       </c>
     </row>
     <row r="46">
@@ -1435,19 +1435,19 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>0.3636363446712494</v>
+        <v>0</v>
       </c>
       <c r="C46" t="n">
-        <v>0.1176470592617989</v>
+        <v>0</v>
       </c>
       <c r="D46" t="n">
-        <v>0.9970847964286804</v>
+        <v>1</v>
       </c>
       <c r="E46" t="n">
-        <v>0.1777773946523666</v>
+        <v>0</v>
       </c>
       <c r="F46" t="n">
-        <v>0.5585470199584961</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="47">
@@ -1457,19 +1457,19 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>0.935258150100708</v>
+        <v>1</v>
       </c>
       <c r="C47" t="n">
-        <v>0.8556617498397827</v>
+        <v>1</v>
       </c>
       <c r="D47" t="n">
-        <v>0.8220926523208618</v>
+        <v>1</v>
       </c>
       <c r="E47" t="n">
-        <v>0.8936906456947327</v>
+        <v>0.9999995231628418</v>
       </c>
       <c r="F47" t="n">
-        <v>0.7225183844566345</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="48">
@@ -1479,19 +1479,19 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>0.3549663722515106</v>
+        <v>0</v>
       </c>
       <c r="C48" t="n">
-        <v>0.6056718230247498</v>
+        <v>0</v>
       </c>
       <c r="D48" t="n">
-        <v>0.8255594372749329</v>
+        <v>1</v>
       </c>
       <c r="E48" t="n">
-        <v>0.4476043283939362</v>
+        <v>0</v>
       </c>
       <c r="F48" t="n">
-        <v>0.7301394939422607</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="49">
@@ -1507,13 +1507,13 @@
         <v>0</v>
       </c>
       <c r="D49" t="n">
-        <v>0.9928301572799683</v>
+        <v>1</v>
       </c>
       <c r="E49" t="n">
         <v>0</v>
       </c>
       <c r="F49" t="n">
-        <v>0.4997620284557343</v>
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>